<commit_message>
final update + handin fodler
</commit_message>
<xml_diff>
--- a/Assignment_01/01_04/ListOfBooks.xlsx
+++ b/Assignment_01/01_04/ListOfBooks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felixwaldschock/Documents/gits/Chalmers_TME286_IntelligentAgents/Assignment_01/01_04/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{76CB515A-F8CF-2B49-AAAF-C2DDD90710DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D935323-AE2A-D14D-A7F3-E07D20F62428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13720" yWindow="860" windowWidth="20480" windowHeight="19940" xr2:uid="{FF2F918C-C965-E24D-A4DC-54CC10B98BD1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="119">
   <si>
     <t>A Check-List of the Birds of Idaho txt</t>
   </si>
@@ -327,13 +327,79 @@
   </si>
   <si>
     <t>Alexandre Dumas</t>
+  </si>
+  <si>
+    <t>Most likely unigrams</t>
+  </si>
+  <si>
+    <t>Most likely bigrams</t>
+  </si>
+  <si>
+    <t>Most likely trigrams</t>
+  </si>
+  <si>
+    <t>unigram</t>
+  </si>
+  <si>
+    <t>FPMI</t>
+  </si>
+  <si>
+    <t>trigram</t>
+  </si>
+  <si>
+    <t>bigrams</t>
+  </si>
+  <si>
+    <t>the</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>and</t>
+  </si>
+  <si>
+    <t>of</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">of the </t>
+  </si>
+  <si>
+    <t xml:space="preserve">. the </t>
+  </si>
+  <si>
+    <t xml:space="preserve">. i </t>
+  </si>
+  <si>
+    <t xml:space="preserve">. and </t>
+  </si>
+  <si>
+    <t>in the</t>
+  </si>
+  <si>
+    <t>. and the</t>
+  </si>
+  <si>
+    <t xml:space="preserve">. it is </t>
+  </si>
+  <si>
+    <t xml:space="preserve">of the lord </t>
+  </si>
+  <si>
+    <t xml:space="preserve">the son of </t>
+  </si>
+  <si>
+    <t xml:space="preserve">out of the </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -359,6 +425,12 @@
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -380,11 +452,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -699,10 +772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1D9B430-1667-F745-BDE2-519B572C4003}">
-  <dimension ref="A1:C71"/>
+  <dimension ref="A1:K71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="139" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:B71"/>
+    <sheetView tabSelected="1" topLeftCell="D34" zoomScale="139" workbookViewId="0">
+      <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -710,6 +783,7 @@
     <col min="1" max="1" width="62.1640625" customWidth="1"/>
     <col min="2" max="2" width="28.5" customWidth="1"/>
     <col min="3" max="3" width="23.1640625" customWidth="1"/>
+    <col min="10" max="10" width="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -878,17 +952,68 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F35" t="s">
+        <v>97</v>
+      </c>
+      <c r="H35" t="s">
+        <v>98</v>
+      </c>
+      <c r="J35" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F36" t="s">
+        <v>100</v>
+      </c>
+      <c r="G36" t="s">
+        <v>101</v>
+      </c>
+      <c r="H36" t="s">
+        <v>103</v>
+      </c>
+      <c r="I36" t="s">
+        <v>101</v>
+      </c>
+      <c r="J36" t="s">
+        <v>102</v>
+      </c>
+      <c r="K36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F37" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G37">
+        <v>50876</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="I37">
+        <v>6651</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="K37">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>33</v>
       </c>
@@ -898,8 +1023,26 @@
       <c r="C38" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F38" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="G38">
+        <v>49836</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="I38">
+        <v>4099</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="K38">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -909,8 +1052,26 @@
       <c r="C39" s="2">
         <v>1928</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F39" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G39">
+        <v>32774</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="I39">
+        <v>2953</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="K39">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -920,8 +1081,26 @@
       <c r="C40" s="2">
         <v>1928</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F40" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="G40">
+        <v>29508</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="I40">
+        <v>2765</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="K40">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -931,8 +1110,26 @@
       <c r="C41" s="2">
         <v>1938</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F41" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="G41">
+        <v>22812</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="I41">
+        <v>2698</v>
+      </c>
+      <c r="J41" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="K41">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>43</v>
       </c>
@@ -943,7 +1140,7 @@
         <v>1845</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>45</v>
       </c>
@@ -954,7 +1151,7 @@
         <v>1902</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>47</v>
       </c>
@@ -965,7 +1162,7 @@
         <v>1875</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>49</v>
       </c>
@@ -975,8 +1172,9 @@
       <c r="C45" s="2">
         <v>1954</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F45" s="4"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>0</v>
       </c>
@@ -986,8 +1184,9 @@
       <c r="C46" s="2">
         <v>1927</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F46" s="4"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>52</v>
       </c>
@@ -997,8 +1196,9 @@
       <c r="C47" s="2">
         <v>1913</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F47" s="4"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>54</v>
       </c>
@@ -1008,8 +1208,9 @@
       <c r="C48" s="2">
         <v>1859</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F48" s="4"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>56</v>
       </c>
@@ -1019,8 +1220,9 @@
       <c r="C49" s="2">
         <v>1912</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F49" s="4"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>58</v>
       </c>
@@ -1031,7 +1233,7 @@
         <v>1924</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>60</v>
       </c>
@@ -1042,7 +1244,7 @@
         <v>1958</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>1</v>
       </c>
@@ -1053,7 +1255,7 @@
         <v>1958</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>62</v>
       </c>
@@ -1064,7 +1266,7 @@
         <v>1958</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>63</v>
       </c>
@@ -1075,7 +1277,7 @@
         <v>1926</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>65</v>
       </c>
@@ -1086,7 +1288,7 @@
         <v>1948</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>67</v>
       </c>
@@ -1097,7 +1299,7 @@
         <v>1915</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>69</v>
       </c>
@@ -1108,7 +1310,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>71</v>
       </c>
@@ -1119,7 +1321,7 @@
         <v>1853</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>73</v>
       </c>
@@ -1130,7 +1332,7 @@
         <v>1818</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>75</v>
       </c>
@@ -1141,7 +1343,7 @@
         <v>1749</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>18</v>
       </c>
@@ -1152,7 +1354,7 @@
         <v>1868</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>78</v>
       </c>
@@ -1163,7 +1365,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>81</v>
       </c>
@@ -1174,7 +1376,7 @@
         <v>1851</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>83</v>
       </c>

</xml_diff>